<commit_message>
preparando para carregar as variáveis das tags
</commit_message>
<xml_diff>
--- a/Codes/ImdbCrawler/CSV files/Análise Tags Discretização.xlsx
+++ b/Codes/ImdbCrawler/CSV files/Análise Tags Discretização.xlsx
@@ -420,8 +420,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -449,8 +457,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,6 +1182,7 @@
       <c r="S11">
         <v>293</v>
       </c>
+      <c r="T11" s="1"/>
       <c r="U11" t="s">
         <v>107</v>
       </c>
@@ -1718,5 +1728,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
buscand as variáveis das tags nos filmes :)
</commit_message>
<xml_diff>
--- a/Codes/ImdbCrawler/CSV files/Análise Tags Discretização.xlsx
+++ b/Codes/ImdbCrawler/CSV files/Análise Tags Discretização.xlsx
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="N7" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>